<commit_message>
rework configuration settings and middleware to support Enabled property
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\DbContextInterceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3A9A9-1F43-4A1A-98AC-CC91E2A5E3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E5B214-A56D-47C7-BF61-E2D6BA255A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="22">
   <si>
     <t>ProjectName</t>
   </si>
@@ -63,30 +63,12 @@
     <t>C</t>
   </si>
   <si>
-    <t>header*X-UserScope=ABC&amp;header*X-Role=admin&amp;header*X-User=moe@stooges.org</t>
-  </si>
-  <si>
     <t>DbContextInterceptorApi</t>
   </si>
   <si>
     <t>PersonController</t>
   </si>
   <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>Headers1</t>
-  </si>
-  <si>
-    <t>Input1</t>
-  </si>
-  <si>
-    <t>Headers2</t>
-  </si>
-  <si>
-    <t>Expected2</t>
-  </si>
-  <si>
     <t>PositionController</t>
   </si>
   <si>
@@ -97,6 +79,24 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>CUD</t>
+  </si>
+  <si>
+    <t>CreateInput</t>
+  </si>
+  <si>
+    <t>UpdateInput</t>
+  </si>
+  <si>
+    <t>CreateExpected</t>
+  </si>
+  <si>
+    <t>UpdateExpected</t>
+  </si>
+  <si>
+    <t>DeleteExpected</t>
   </si>
 </sst>
 </file>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -462,7 +462,7 @@
     <col min="3" max="3" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.06640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
@@ -492,428 +492,512 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="1" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="1" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ongoing testing work ... ongoing work on DbContextInterceptorMiddleware tests
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\DbContextInterceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E5B214-A56D-47C7-BF61-E2D6BA255A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4296FFB1-4ED2-498E-BF02-8259359EDD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="210" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="39">
   <si>
     <t>ProjectName</t>
   </si>
@@ -60,43 +60,94 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>DbContextInterceptorApi</t>
   </si>
   <si>
     <t>PersonController</t>
   </si>
   <si>
-    <t>PositionController</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>CUD</t>
   </si>
   <si>
-    <t>CreateInput</t>
-  </si>
-  <si>
-    <t>UpdateInput</t>
-  </si>
-  <si>
-    <t>CreateExpected</t>
-  </si>
-  <si>
-    <t>UpdateExpected</t>
-  </si>
-  <si>
-    <t>DeleteExpected</t>
+    <t>ResetExpected</t>
+  </si>
+  <si>
+    <t>{"Id":-999005,"Name":"Marcia"}</t>
+  </si>
+  <si>
+    <t>{"Id":-999005,"Name":"Peter"}</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}]</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>CreateInput1</t>
+  </si>
+  <si>
+    <t>CreateInput2a</t>
+  </si>
+  <si>
+    <t>CreateInput2b</t>
+  </si>
+  <si>
+    <t>CreateExpected1</t>
+  </si>
+  <si>
+    <t>CreateExpected2</t>
+  </si>
+  <si>
+    <t>{"Id":-999006,"Name":"Jan"}</t>
+  </si>
+  <si>
+    <t>moe</t>
+  </si>
+  <si>
+    <t>larry</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Marcia", "SysUser":"moe"}]</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Peter", "SysUser":"larry"}, {"Id":-999006, "Name":"Jan", "SysUser":"larry"}]</t>
+  </si>
+  <si>
+    <t>UpdateInput1</t>
+  </si>
+  <si>
+    <t>UpdateInput2</t>
+  </si>
+  <si>
+    <t>{"Id":-999006,"Name":"Cindy"}</t>
+  </si>
+  <si>
+    <t>{"Id":-999005,"Name":"Alice"}</t>
+  </si>
+  <si>
+    <t>UpdateExpected1</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Alice", "SysUser":"moe"}]</t>
+  </si>
+  <si>
+    <t>UpdateExpected2</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Peter", "SysUser":"larry"}, {"Id":-999006, "Name":"Cindy", "SysUser":"larry"}]</t>
+  </si>
+  <si>
+    <t>DeleteExpected1</t>
+  </si>
+  <si>
+    <t>DeleteExpected2a</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999006, "Name":"Cindy", "SysUser":"larry"}]</t>
   </si>
 </sst>
 </file>
@@ -449,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -462,7 +513,7 @@
     <col min="3" max="3" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="14.06640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" style="1" customWidth="1"/>
     <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
@@ -492,47 +543,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -540,464 +597,508 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ongoing middleware testing work ... ongoing setup work for testing DbContextInterceptorMiddleware
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\DbContextInterceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AAE9E3-15A0-4F40-A254-79BBA4B3F7BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88499A7A-1CA1-4978-A1C9-43B9446E27BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="25080" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="45">
   <si>
     <t>ProjectName</t>
   </si>
@@ -69,12 +69,6 @@
     <t>CUD</t>
   </si>
   <si>
-    <t>{"Id":-999005,"Name":"Marcia"}</t>
-  </si>
-  <si>
-    <t>{"Id":-999005,"Name":"Peter"}</t>
-  </si>
-  <si>
     <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}]</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>CreateExpected1</t>
   </si>
   <si>
-    <t>{"Id":-999006,"Name":"Jan"}</t>
-  </si>
-  <si>
     <t>moe</t>
   </si>
   <si>
@@ -96,27 +87,12 @@
     <t>UpdateInput1</t>
   </si>
   <si>
-    <t>{"Id":-999006,"Name":"Cindy"}</t>
-  </si>
-  <si>
-    <t>{"Id":-999005,"Name":"Alice"}</t>
-  </si>
-  <si>
     <t>UpdateExpected1</t>
   </si>
   <si>
     <t>DeleteExpected1</t>
   </si>
   <si>
-    <t>CreateInput1a</t>
-  </si>
-  <si>
-    <t>CreateInput1b</t>
-  </si>
-  <si>
-    <t>{"Id":-999007,"Name":"Bobby"}</t>
-  </si>
-  <si>
     <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999002, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999003, "Name":"Greg", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Marcia", "SysUser":"moe"}, {"Id":-999007, "Name":"Bobby", "SysUser":"moe"}]</t>
   </si>
   <si>
@@ -138,12 +114,6 @@
     <t>User0</t>
   </si>
   <si>
-    <t>CreateInput0a</t>
-  </si>
-  <si>
-    <t>CreateInput0b</t>
-  </si>
-  <si>
     <t>CreateExpected0</t>
   </si>
   <si>
@@ -157,6 +127,45 @@
   </si>
   <si>
     <t>BaseExpected</t>
+  </si>
+  <si>
+    <t>CreateInput0</t>
+  </si>
+  <si>
+    <t>[{"Id":-999005,"Name":"Marcia"},{"Id":-999007,"Name":"Bobby"}]</t>
+  </si>
+  <si>
+    <t>CreateInput1</t>
+  </si>
+  <si>
+    <t>[{"Id":-999005,"Name":"Peter"},{"Id":-999006,"Name":"Jan"}]</t>
+  </si>
+  <si>
+    <t>[{"Id":-999005,"Name":"Alice"}]</t>
+  </si>
+  <si>
+    <t>[{"Id":-999006,"Name":"Cindy"}]</t>
+  </si>
+  <si>
+    <t>CreateInputs0</t>
+  </si>
+  <si>
+    <t>CreateInputs1</t>
+  </si>
+  <si>
+    <t>UpdateInputs0</t>
+  </si>
+  <si>
+    <t>UpdateInputs1</t>
+  </si>
+  <si>
+    <t>DeleteIds0</t>
+  </si>
+  <si>
+    <t>DeleteIds1</t>
+  </si>
+  <si>
+    <t>[-999005]</t>
   </si>
 </sst>
 </file>
@@ -512,7 +521,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +573,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,10 +593,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -604,10 +613,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -624,10 +633,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -644,10 +653,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,10 +673,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,10 +693,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -704,10 +713,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -724,10 +733,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -744,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>22</v>
@@ -764,10 +773,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -784,10 +793,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -804,10 +813,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -824,10 +833,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,10 +853,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -864,10 +873,10 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -884,10 +893,10 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,10 +913,10 @@
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,10 +933,10 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -944,10 +953,10 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,10 +973,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1004,10 +1013,10 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,10 +1033,10 @@
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>22</v>
@@ -1064,10 +1073,10 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1084,10 +1093,10 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,10 +1113,10 @@
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1124,10 +1133,10 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,10 +1153,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DbContextInterceptorMiddleware tests passing, but only if SqlServer and InMemory tests are run separately.  The InMemory tests hang if run together.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\DbContextInterceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88499A7A-1CA1-4978-A1C9-43B9446E27BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6CADFC-63E2-4D22-9AAA-958E3B6EB10B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="41">
   <si>
     <t>ProjectName</t>
   </si>
@@ -84,9 +84,6 @@
     <t>larry</t>
   </si>
   <si>
-    <t>UpdateInput1</t>
-  </si>
-  <si>
     <t>UpdateExpected1</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>CreateExpected0</t>
   </si>
   <si>
-    <t>UpdateInput0</t>
-  </si>
-  <si>
     <t>UpdateExpected0</t>
   </si>
   <si>
@@ -129,13 +123,7 @@
     <t>BaseExpected</t>
   </si>
   <si>
-    <t>CreateInput0</t>
-  </si>
-  <si>
     <t>[{"Id":-999005,"Name":"Marcia"},{"Id":-999007,"Name":"Bobby"}]</t>
-  </si>
-  <si>
-    <t>CreateInput1</t>
   </si>
   <si>
     <t>[{"Id":-999005,"Name":"Peter"},{"Id":-999006,"Name":"Jan"}]</t>
@@ -520,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -593,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>15</v>
@@ -633,10 +621,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -653,10 +641,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,10 +661,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -696,7 +684,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,10 +701,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -733,10 +721,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -753,10 +741,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -773,10 +761,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,10 +781,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -813,10 +801,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -833,10 +821,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -853,10 +841,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
@@ -893,7 +881,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>15</v>
@@ -933,10 +921,10 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -953,10 +941,10 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -996,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1013,10 +1001,10 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1033,10 +1021,10 @@
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,10 +1041,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1073,10 +1061,10 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,10 +1081,10 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,10 +1101,10 @@
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1133,10 +1121,10 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,10 +1141,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DbContextInterceptorMiddleware tests now passing.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/DbContextInterceptor/TestJson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\DbContextInterceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6CADFC-63E2-4D22-9AAA-958E3B6EB10B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A8FF8-DF1E-46B0-9895-5D3005A0894C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>CUD</t>
   </si>
   <si>
-    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999005, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999005, "Name":"Greg", "SysUser":"jack@hill.org"}]</t>
-  </si>
-  <si>
     <t>User1</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>[-999005]</t>
+  </si>
+  <si>
+    <t>[{"Id":-999001, "Name":"Mike", "SysUser":"jack@hill.org"}, {"Id":-999002, "Name":"Carol", "SysUser":"jill@hill.org"}, {"Id":-999003, "Name":"Greg", "SysUser":"jack@hill.org"}]</t>
   </si>
 </sst>
 </file>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +561,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -581,10 +581,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -601,10 +601,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -621,10 +621,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -641,10 +641,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,10 +661,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -681,10 +681,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -701,10 +701,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -721,10 +721,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -741,10 +741,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -761,10 +761,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -781,10 +781,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -801,10 +801,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -821,10 +821,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,10 +841,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -861,10 +861,10 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,10 +881,10 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,10 +901,10 @@
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -921,10 +921,10 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -941,10 +941,10 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -961,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -981,10 +981,10 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,10 +1001,10 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1021,10 +1021,10 @@
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1041,10 +1041,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,10 +1061,10 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1081,10 +1081,10 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,10 +1101,10 @@
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1121,10 +1121,10 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,10 +1141,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>